<commit_message>
feat: hw revision 1.0.3
</commit_message>
<xml_diff>
--- a/hardware/gas_nrf52832/pcb/2차_Rev1.0.2(4L)/SMT/bom.xlsx
+++ b/hardware/gas_nrf52832/pcb/2차_Rev1.0.2(4L)/SMT/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradkim06/hhs/docker/work/gas_ces/hardware/gas_nrf52832/pcb/SMT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradkim06/hhs/docker/work/gas_ces/hardware/gas_nrf52832/pcb/2차_Rev1.0.2(4L)/SMT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{17914038-18B0-2B43-83C6-FEFA7178C841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{863AC7DE-A0D3-FC48-88E7-6D698013BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="500" windowWidth="41440" windowHeight="28300" xr2:uid="{42974862-43F6-CA4D-BBAF-800A9D907AA8}"/>
+    <workbookView xWindow="3200" yWindow="500" windowWidth="47980" windowHeight="28300" xr2:uid="{42974862-43F6-CA4D-BBAF-800A9D907AA8}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="214" uniqueCount="145">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="215" uniqueCount="146">
   <si>
     <t>Reference</t>
   </si>
@@ -462,6 +462,10 @@
   </si>
   <si>
     <t>C3,C7,C8,C13,C20,C21</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD-4</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1055,14 +1059,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1443,7 +1441,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1484,785 +1482,789 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1">
-      <c r="A3" s="2" t="s">
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1">
-      <c r="A4" s="2" t="s">
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>126</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1">
-      <c r="A5" s="1" t="s">
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1">
-      <c r="A6" s="1" t="s">
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>128</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1">
-      <c r="A7" s="2" t="s">
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1">
-      <c r="A8" s="2" t="s">
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1">
-      <c r="A9" s="2" t="s">
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1">
-      <c r="A10" s="2" t="s">
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1">
-      <c r="A11" s="2" t="s">
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>3</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1">
-      <c r="A12" s="2" t="s">
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1">
-      <c r="A13" s="2" t="s">
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="2" customFormat="1">
-      <c r="A14" s="2" t="s">
+      <c r="G13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>130</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="2" customFormat="1">
-      <c r="A15" s="2" t="s">
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" t="s">
         <v>131</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="2" customFormat="1">
-      <c r="A16" s="2" t="s">
+      <c r="H15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" t="s">
         <v>129</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="2" customFormat="1">
-      <c r="A17" s="2" t="s">
+      <c r="H16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" t="s">
         <v>76</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1">
-      <c r="A18" s="2" t="s">
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" t="s">
         <v>132</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="1" customFormat="1">
-      <c r="A19" s="1" t="s">
+      <c r="H18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" t="s">
         <v>133</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="1" customFormat="1">
-      <c r="A20" s="1" t="s">
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" t="s">
         <v>140</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="2" customFormat="1">
-      <c r="A21" s="2" t="s">
+      <c r="H20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" t="s">
         <v>134</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="2" customFormat="1">
-      <c r="A22" s="2" t="s">
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" t="s">
         <v>135</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="1" customFormat="1">
-      <c r="A23" s="1" t="s">
+      <c r="H22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" t="s">
         <v>141</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="2" customFormat="1">
-      <c r="A24" s="2" t="s">
+      <c r="H23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>100</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" t="s">
         <v>99</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" t="s">
         <v>136</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="2" customFormat="1">
-      <c r="A25" s="2" t="s">
+      <c r="H24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" t="s">
         <v>137</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="2" customFormat="1">
-      <c r="A26" s="2" t="s">
+      <c r="H25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>10</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>3</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" t="s">
         <v>138</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="2" customFormat="1">
-      <c r="A27" s="2" t="s">
+      <c r="H26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" t="s">
         <v>139</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="1" customFormat="1">
-      <c r="A28" s="1" t="s">
+      <c r="H27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>150</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>83</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" t="s">
         <v>142</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="1" customFormat="1">
-      <c r="A29" s="1" t="s">
+      <c r="H28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>2</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>112</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" t="s">
         <v>143</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="2" customFormat="1">
-      <c r="A30" s="2" t="s">
+      <c r="H29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" t="s">
         <v>116</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" t="s">
         <v>117</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="2" customFormat="1">
-      <c r="A31" s="2" t="s">
+      <c r="H30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" t="s">
         <v>120</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" t="s">
         <v>122</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" t="s">
         <v>123</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>